<commit_message>
Removed level specification in instructions; fixed small errors
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/E.US-EIA_inventory_CEDSsec-instructions.xlsx
+++ b/input/extension/user-defined-energy/E.US-EIA_inventory_CEDSsec-instructions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="20">
   <si>
     <t>iso</t>
   </si>
@@ -42,22 +42,7 @@
     <t>priority</t>
   </si>
   <si>
-    <t>L1_agg_fuel</t>
-  </si>
-  <si>
-    <t>L2_CEDS_fuel</t>
-  </si>
-  <si>
-    <t>L3_agg_sector</t>
-  </si>
-  <si>
-    <t>L4_CEDS_sector</t>
-  </si>
-  <si>
     <t>override_normalization</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>usa</t>
@@ -421,26 +406,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -454,31 +439,19 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>1949</v>
@@ -489,114 +462,99 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1949</v>
+      </c>
+      <c r="F3">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>1949</v>
-      </c>
-      <c r="F3">
-        <v>2016</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1949</v>
+      </c>
+      <c r="F4">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1949</v>
+      </c>
+      <c r="F5">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1949</v>
+      </c>
+      <c r="F6">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>1949</v>
-      </c>
-      <c r="F4">
-        <v>2016</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1949</v>
-      </c>
-      <c r="F5">
-        <v>2016</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>1949</v>
-      </c>
-      <c r="F6">
-        <v>2016</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>1949</v>
@@ -604,22 +562,19 @@
       <c r="F7">
         <v>2007</v>
       </c>
-      <c r="J7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>1949</v>
@@ -627,31 +582,25 @@
       <c r="F8">
         <v>2016</v>
       </c>
-      <c r="J8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>1949</v>
       </c>
       <c r="F9">
         <v>2016</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -674,13 +623,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -689,27 +638,27 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>1949</v>
@@ -718,21 +667,21 @@
         <v>2016</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>1949</v>
@@ -741,21 +690,21 @@
         <v>2016</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>1949</v>
@@ -764,21 +713,21 @@
         <v>2016</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>1949</v>
@@ -787,44 +736,44 @@
         <v>2016</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1949</v>
+      </c>
+      <c r="F6">
+        <v>2016</v>
+      </c>
+      <c r="I6" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>1949</v>
-      </c>
-      <c r="F6">
-        <v>2016</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>1949</v>
@@ -833,53 +782,53 @@
         <v>2007</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>1949</v>
+      </c>
+      <c r="F8">
+        <v>2016</v>
+      </c>
+      <c r="I8" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8">
-        <v>1949</v>
-      </c>
-      <c r="F8">
-        <v>2016</v>
-      </c>
-      <c r="I8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>1949</v>
+      </c>
+      <c r="F9">
+        <v>2016</v>
+      </c>
+      <c r="I9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <v>1949</v>
-      </c>
-      <c r="F9">
-        <v>2016</v>
-      </c>
-      <c r="I9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>